<commit_message>
Refactored Full Booking journey
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager_Full_Auction_Journey.xlsx
+++ b/src/test/resources/Run_Manager_Full_Auction_Journey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\New_Sakani_TST_Git\Sakani_TST_New\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAD9556-B96C-4C04-9246-D13A85945D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EEE4C8-2800-4132-BA3A-29BDD3B5BEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2148" windowWidth="18756" windowHeight="10092" tabRatio="697" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="697" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuiteDetails" sheetId="1" r:id="rId1"/>
@@ -2826,10 +2826,10 @@
   <dimension ref="A1:M158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D141" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J145" sqref="J145:J146"/>
+      <selection pane="bottomRight" activeCell="A119" sqref="A119:XFD150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="30" customHeight="1"/>
@@ -8979,7 +8979,7 @@
   <conditionalFormatting sqref="E1:F1">
     <cfRule type="duplicateValues" dxfId="2" priority="366"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J88 J90:J106 J108:J116 J152:J158 J118:J150">
+  <conditionalFormatting sqref="J3:J88 J90:J106 J108:J116 J118:J150 J152:J158">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>

</xml_diff>